<commit_message>
Finish excel operator reading
</commit_message>
<xml_diff>
--- a/data/operator_def_1.xlsx
+++ b/data/operator_def_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakeboersma/School/AI Project/ai-project-post-break/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F22B511-20A4-1146-82B3-84CAA734BBA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB1338B-615E-624B-AAD9-6A452D95971D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2840" yWindow="3500" windowWidth="23620" windowHeight="15460" xr2:uid="{ED844C13-9B21-4E40-B03F-93EF884CFD31}"/>
+    <workbookView xWindow="2840" yWindow="2540" windowWidth="23620" windowHeight="15460" xr2:uid="{ED844C13-9B21-4E40-B03F-93EF884CFD31}"/>
   </bookViews>
   <sheets>
     <sheet name="Operators" sheetId="2" r:id="rId1"/>
@@ -45,9 +45,6 @@
     <t>electronics_transform</t>
   </si>
   <si>
-    <t>?AIk &lt;= ?C(?Rk)</t>
-  </si>
-  <si>
     <t>housing_transform</t>
   </si>
   <si>
@@ -58,6 +55,9 @@
   </si>
   <si>
     <t>"('TRANSFORM', '?C', ('INPUTS', ('R1', 3), ('R2', 2), ('R21', 2)), ('OUTPUTS', ('R22', 2), ('R22’, 2), ('R1', 3)))"</t>
+  </si>
+  <si>
+    <t>?ARk &lt;= ?C(?Rk)</t>
   </si>
 </sst>
 </file>
@@ -444,7 +444,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -470,7 +470,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>3</v>
@@ -481,7 +481,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
@@ -489,13 +489,13 @@
     </row>
     <row r="4" spans="1:3" s="1" customFormat="1" ht="34">
       <c r="A4" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="1" customFormat="1">

</xml_diff>